<commit_message>
Implemented MeanCenter and Normalize functions Need to fix parsing to handle needs of stat and xform ops
</commit_message>
<xml_diff>
--- a/test/StatGoldStd.xlsx
+++ b/test/StatGoldStd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21800" yWindow="4820" windowWidth="16780" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="13000" yWindow="2020" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t xml:space="preserve">Mean: </t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>Correlation</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Statistic</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Mean Center</t>
+  </si>
+  <si>
+    <t>Normalize</t>
   </si>
 </sst>
 </file>
@@ -429,175 +447,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="18.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1">
-        <v>3096951</v>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>3.68</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <f>AVERAGE(A:A)</f>
-        <v>2053751.8333333333</v>
-      </c>
-      <c r="F1">
+        <v>3.0516666666666672</v>
+      </c>
+      <c r="F2">
+        <f>STANDARDIZE(A2,D$2,D$4)</f>
+        <v>0.35593272129909609</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G1">
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="J1">
-        <f>SLOPE(G:G,F:F)</f>
+      <c r="K2">
+        <f>SLOPE(H:H,G:G)</f>
         <v>1.1486486486486487</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1123560</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>1.28</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <f>_xlfn.STDEV.P(A:A)</f>
-        <v>1840895.0931444932</v>
-      </c>
-      <c r="F2">
+        <v>1.6115046454237176</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="0">STANDARDIZE(A3,D$2,D$4)</f>
+        <v>-1.003598097456073</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="J2">
-        <f>INTERCEPT(G:G,F:F)</f>
+      <c r="K3">
+        <f>INTERCEPT(H:H,G:G)</f>
         <v>-0.21621621621621623</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>5725983</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>1.84</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <f>_xlfn.STDEV.S(A:A)</f>
-        <v>2016599.5370316256</v>
-      </c>
-      <c r="F3">
+        <v>1.7653148916458685</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>-0.68637423974653344</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="H4">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="J3">
-        <f>CORREL(F:F,G:G)</f>
+      <c r="K4">
+        <f>CORREL(G:G,H:H)</f>
         <v>0.98810492932246385</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>918959</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>3.68</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <f>_xlfn.VAR.P(A:A)</f>
-        <v>3388894743963.4722</v>
-      </c>
-      <c r="F4">
+        <v>2.5969472222222216</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.35593272129909609</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="G4">
+      <c r="H5">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>945761</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>1.83</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <f>MIN(A:A)</f>
-        <v>511297</v>
-      </c>
-      <c r="F5">
+        <v>1.28</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-0.69203895149134664</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="G5">
+      <c r="H6">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>511297</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f>MAX(A:A)</f>
-        <v>5725983</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7">
-        <f>D6-D5</f>
-        <v>5214686</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.6701458460957594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>D7-D6</f>
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <f>COUNT(A:A)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="C9" s="1" t="s">
+    <row r="10" spans="1:11">
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <f>SKEW(A:A)</f>
-        <v>1.5861833067973581</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="C10" s="1" t="s">
+        <v>0.92497431632438487</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.STDEV.S(F2:F7)</f>
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f>KURT(A:A)</f>
-        <v>1.9027097778139002</v>
+        <v>0.24499009527889193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>